<commit_message>
Aanpassing homepagina + todo
</commit_message>
<xml_diff>
--- a/To Do/Vanlessen Jeroen.xlsx
+++ b/To Do/Vanlessen Jeroen.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="42">
   <si>
     <t>Prioriteit:</t>
   </si>
@@ -137,6 +137,9 @@
   </si>
   <si>
     <t>HTML 5 &amp; JSP tutorials</t>
+  </si>
+  <si>
+    <t>7 uur</t>
   </si>
 </sst>
 </file>
@@ -874,7 +877,7 @@
   <dimension ref="A1:K41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1069,7 +1072,9 @@
       <c r="B7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="3"/>
+      <c r="C7" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="E7" s="1">
         <v>1</v>
       </c>

</xml_diff>